<commit_message>
Adjust filenames for relative path
</commit_message>
<xml_diff>
--- a/Examples/Studio/ellipsoid.xlsx
+++ b/Examples/Studio/ellipsoid.xlsx
@@ -1,30 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amorris/sci/shapeworks/code/Examples/Studio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38714AF-CF9D-434D-8359-70BF338A57D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="groom" sheetId="13" r:id="rId2"/>
-    <sheet name="optimize" sheetId="14" r:id="rId3"/>
-    <sheet name="analysis" sheetId="15" r:id="rId4"/>
-    <sheet name="studio" sheetId="16" r:id="rId5"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="groom" sheetId="21" r:id="rId2"/>
+    <sheet name="optimize" sheetId="22" r:id="rId3"/>
+    <sheet name="analysis" sheetId="23" r:id="rId4"/>
+    <sheet name="studio" sheetId="24" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>segmentation_file</t>
   </si>
@@ -180,12 +179,48 @@
   </si>
   <si>
     <t>ellipsoid_2.nrrd</t>
+  </si>
+  <si>
+    <t>groom</t>
+  </si>
+  <si>
+    <t>Groomed</t>
+  </si>
+  <si>
+    <t>groomed_file</t>
+  </si>
+  <si>
+    <t>ellipsoid_1_DT.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_2_DT.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_3_DT.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_4_DT.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_5_DT.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_6_DT.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_7_DT.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_8_DT.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_9_DT.nrrd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -226,9 +261,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -496,8 +528,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
@@ -508,54 +540,84 @@
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -563,15 +625,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -579,7 +638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -587,7 +646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -595,7 +654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -603,7 +662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -611,7 +670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -619,7 +678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -627,7 +686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -635,7 +694,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -643,7 +702,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -651,7 +710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -660,19 +719,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -680,7 +735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -688,7 +743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -696,7 +751,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -704,7 +759,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -712,7 +767,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -720,7 +775,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -728,7 +783,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -737,19 +792,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -757,7 +808,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -765,7 +816,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -773,7 +824,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -782,19 +833,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -802,7 +849,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -810,23 +857,23 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -835,6 +882,5 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Set a project paramater page with version=1
</commit_message>
<xml_diff>
--- a/Examples/Studio/ellipsoid.xlsx
+++ b/Examples/Studio/ellipsoid.xlsx
@@ -13,17 +13,17 @@
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="groom" sheetId="21" r:id="rId2"/>
-    <sheet name="optimize" sheetId="22" r:id="rId3"/>
-    <sheet name="analysis" sheetId="23" r:id="rId4"/>
-    <sheet name="studio" sheetId="24" r:id="rId5"/>
+    <sheet name="groom" sheetId="29" r:id="rId2"/>
+    <sheet name="optimize" sheetId="30" r:id="rId3"/>
+    <sheet name="analysis" sheetId="31" r:id="rId4"/>
+    <sheet name="studio" sheetId="32" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>segmentation_file</t>
   </si>
@@ -148,73 +148,43 @@
     <t>zoom_state</t>
   </si>
   <si>
+    <t>ellipsoid_1.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_9.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_8.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_7.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_6.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_5.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_4.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_3.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_2.nrrd</t>
+  </si>
+  <si>
+    <t>groom</t>
+  </si>
+  <si>
+    <t>Groomed</t>
+  </si>
+  <si>
     <t>data</t>
   </si>
   <si>
     <t>Original</t>
-  </si>
-  <si>
-    <t>ellipsoid_1.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_9.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_8.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_7.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_6.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_5.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_4.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_3.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_2.nrrd</t>
-  </si>
-  <si>
-    <t>groom</t>
-  </si>
-  <si>
-    <t>Groomed</t>
-  </si>
-  <si>
-    <t>groomed_file</t>
-  </si>
-  <si>
-    <t>ellipsoid_1_DT.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_2_DT.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_3_DT.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_4_DT.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_5_DT.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_6_DT.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_7_DT.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_8_DT.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_9_DT.nrrd</t>
   </si>
 </sst>
 </file>
@@ -529,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,84 +510,54 @@
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -625,7 +565,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -722,7 +662,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B8"/>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -795,7 +735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -836,7 +776,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B5"/>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>